<commit_message>
the upload and download excel done (Test Case ready)
</commit_message>
<xml_diff>
--- a/server/excel_template/UserInfo.xlsx
+++ b/server/excel_template/UserInfo.xlsx
@@ -1,63 +1,272 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelvin_chang\Desktop\IVE_FYP\ive-fyp\server\excel_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kahei\Desktop\ive-fyp\server\excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6335DA-8A5F-43C2-A215-B50BB930EB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C209DA-7544-4E01-B95F-61810416B211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DOIvfQ4H/zfRSsWOYGsI6nUwnCjENGx5Aq9158D/FDDCDxdvcceqdHHCwa/x/7Y8qnwDwKGrQSo6t1CRmKsfGw==" workbookSaltValue="TnHeOaizAVLGloqR/V82lw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3768" yWindow="19092" windowWidth="23256" windowHeight="12456" xr2:uid="{9E734FD6-9546-4BDD-A69B-D0F258AE635A}"/>
   </bookViews>
   <sheets>
     <sheet name="Add User" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>英文姓名 / Name</t>
-  </si>
-  <si>
-    <t>電話號碼 (mobile)</t>
-  </si>
-  <si>
-    <t>電郵 (Email)</t>
+    <t xml:space="preserve">中文姓名 (Chinese Name) </t>
   </si>
   <si>
     <t>中文地址 (Chinese Address)</t>
   </si>
   <si>
-    <t>英文地址 (Address)</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>為必需填寫</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is required</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">中文姓名 (Chinese Name) </t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>英文姓名 / Name</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>電話號碼 (mobile)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>電郵 (Email)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>英文地址 (Address)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -111,27 +320,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -147,7 +374,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -157,39 +384,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -222,9 +449,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -257,6 +501,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -318,13 +579,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -333,6 +587,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -397,391 +658,424 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EACDB2-A07A-48A0-83EF-940A4459C1B1}">
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.08984375" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="24.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="45.88671875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.08984375" style="3"/>
+    <col min="2" max="2" width="22.36328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.90625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18" style="3" customWidth="1"/>
+    <col min="6" max="6" width="40.7265625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="57.36328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="28.36328125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.08984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A1" s="1"/>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="8"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="E19" s="8"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="E20" s="8"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="E21" s="8"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="E22" s="8"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="E24" s="8"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="E25" s="8"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="E26" s="8"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="E27" s="8"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="E28" s="8"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="E29" s="8"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="E30" s="8"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="E31" s="8"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="SegckFWzd1kbTViUmNfuxNgoavMHjVi7e+GFrUh8hH/kCXcs4TnuoT8eKVHuERB7G97P9P9dNzjyvLnTw3Xrmg==" saltValue="Hw1qPH+zcHBFcTxG95DPpQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please only input letters and spaces!_x000a_請僅輸入英文字母和空格!" sqref="B2:B31" xr:uid="{71F114F4-8C4B-446B-BBCA-CA68DB44C23C}">
+      <formula1>AND(ISTEXT(B2), NOT(ISERROR(MATCH(TRUE, ISNUMBER(FIND(MID(B2,ROW(INDIRECT("1:"&amp;LEN(B2))), 1), "ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz")), 0))))</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" imeMode="off" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please input 8 digit number!_x000a_請輸入八位數字!" sqref="D2:D31" xr:uid="{8F92E5BF-5B18-4226-ABBA-A9AAB5E0B2B9}">
+      <formula1>8</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update the sql and insert user template
</commit_message>
<xml_diff>
--- a/server/excel_template/UserInfo.xlsx
+++ b/server/excel_template/UserInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kahei\Desktop\ive-fyp\server\excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C209DA-7544-4E01-B95F-61810416B211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314FC073-5190-4D74-9997-3AD4B5AB8B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DOIvfQ4H/zfRSsWOYGsI6nUwnCjENGx5Aq9158D/FDDCDxdvcceqdHHCwa/x/7Y8qnwDwKGrQSo6t1CRmKsfGw==" workbookSaltValue="TnHeOaizAVLGloqR/V82lw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="3768" yWindow="19092" windowWidth="23256" windowHeight="12456" xr2:uid="{9E734FD6-9546-4BDD-A69B-D0F258AE635A}"/>
@@ -37,12 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">中文姓名 (Chinese Name) </t>
-  </si>
-  <si>
-    <t>中文地址 (Chinese Address)</t>
   </si>
   <si>
     <r>
@@ -169,31 +166,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>電郵 (Email)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>英文地址 (Address)</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -690,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EACDB2-A07A-48A0-83EF-940A4459C1B1}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.08984375" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -703,34 +675,26 @@
     <col min="3" max="3" width="23.90625" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.54296875" style="3" customWidth="1"/>
     <col min="5" max="5" width="18" style="3" customWidth="1"/>
-    <col min="6" max="6" width="40.7265625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="57.36328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="28.36328125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.08984375" style="3"/>
+    <col min="6" max="6" width="28.36328125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.08984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -738,13 +702,11 @@
       <c r="C2" s="5"/>
       <c r="D2" s="9"/>
       <c r="E2" s="8"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -752,13 +714,11 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F3" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -766,10 +726,8 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -777,10 +735,8 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -788,10 +744,8 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -799,10 +753,8 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -810,10 +762,8 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -821,10 +771,8 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -832,10 +780,8 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -843,10 +789,8 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -854,10 +798,8 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -865,10 +807,8 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -876,10 +816,8 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -887,10 +825,8 @@
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -898,10 +834,8 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -909,10 +843,8 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -920,10 +852,8 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -931,10 +861,8 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -942,10 +870,8 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -953,10 +879,8 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -964,10 +888,8 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -975,10 +897,8 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -986,10 +906,8 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -997,10 +915,8 @@
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1008,10 +924,8 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1019,10 +933,8 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1030,10 +942,8 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1041,10 +951,8 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1052,10 +960,8 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1063,10 +969,9 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="WOrXxJkF6byHuEvu3DDltYPdszCdHdhNkf1GCnBPnMZeWUudfKn2HF1mr+L67qdC7tvTULHuTRmrZhsg3ZGKsQ==" saltValue="A1kANToiXF871/LV/R1ifA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please only input letters and spaces!_x000a_請僅輸入英文字母和空格!" sqref="B2:B31" xr:uid="{71F114F4-8C4B-446B-BBCA-CA68DB44C23C}">

</xml_diff>

<commit_message>
update the submit file function
</commit_message>
<xml_diff>
--- a/server/excel_template/UserInfo.xlsx
+++ b/server/excel_template/UserInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kahei\Desktop\ive-fyp\server\excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C990538-ED82-4615-ABDD-CC316B83515B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBF760F-8A24-4896-8201-F4A0EB02AD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DOIvfQ4H/zfRSsWOYGsI6nUwnCjENGx5Aq9158D/FDDCDxdvcceqdHHCwa/x/7Y8qnwDwKGrQSo6t1CRmKsfGw==" workbookSaltValue="TnHeOaizAVLGloqR/V82lw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{9E734FD6-9546-4BDD-A69B-D0F258AE635A}"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="130">
   <si>
     <t xml:space="preserve">中文姓名 (Chinese Name) </t>
   </si>
@@ -201,6 +201,369 @@
   <si>
     <t>Staff</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lin Huafei</t>
+  </si>
+  <si>
+    <t>林華菲</t>
+  </si>
+  <si>
+    <t>john.doe123@example.com</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Zhang Wenqing</t>
+  </si>
+  <si>
+    <t>張文晴</t>
+  </si>
+  <si>
+    <t>sarah.smith456@example.com</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Qiu Zilu</t>
+  </si>
+  <si>
+    <t>邱梓潞</t>
+  </si>
+  <si>
+    <t>michael.brown789@example.com</t>
+  </si>
+  <si>
+    <t>Li Haixue</t>
+  </si>
+  <si>
+    <t>李海雪</t>
+  </si>
+  <si>
+    <t>emily.jones001@example.com</t>
+  </si>
+  <si>
+    <t>Chen Lungui</t>
+  </si>
+  <si>
+    <t>陳倫貴</t>
+  </si>
+  <si>
+    <t>david.wilson234@example.com</t>
+  </si>
+  <si>
+    <t>Wu Tongye</t>
+  </si>
+  <si>
+    <t>吳彤曄</t>
+  </si>
+  <si>
+    <t>jessica.taylor567@example.com</t>
+  </si>
+  <si>
+    <t>Huang Guoyong</t>
+  </si>
+  <si>
+    <t>黃國庸</t>
+  </si>
+  <si>
+    <t>chris.johnson890@example.com</t>
+  </si>
+  <si>
+    <t>Liu Shengqun</t>
+  </si>
+  <si>
+    <t>劉勝羣</t>
+  </si>
+  <si>
+    <t>katie.miller345@example.com</t>
+  </si>
+  <si>
+    <t>Kim Baehwan</t>
+  </si>
+  <si>
+    <t>金沛煥</t>
+  </si>
+  <si>
+    <t>robert.davis678@example.com</t>
+  </si>
+  <si>
+    <t>Wang Wunan</t>
+  </si>
+  <si>
+    <t>王悟楠</t>
+  </si>
+  <si>
+    <t>laura.garcia012@example.com</t>
+  </si>
+  <si>
+    <t>Chen Chuqun</t>
+  </si>
+  <si>
+    <t>陳楚羣</t>
+  </si>
+  <si>
+    <t>daniel.martinez789@example.com</t>
+  </si>
+  <si>
+    <t>Lin Shirun</t>
+  </si>
+  <si>
+    <t>林實潤</t>
+  </si>
+  <si>
+    <t>amanda.rodriguez234@example.com</t>
+  </si>
+  <si>
+    <t>Zheng Taoshu</t>
+  </si>
+  <si>
+    <t>鄭濤術</t>
+  </si>
+  <si>
+    <t>joshua.lewis456@example.com</t>
+  </si>
+  <si>
+    <t>Huang Baoming</t>
+  </si>
+  <si>
+    <t>黃寶明</t>
+  </si>
+  <si>
+    <t>megan.walker001@example.com</t>
+  </si>
+  <si>
+    <t>Hong Chengya</t>
+  </si>
+  <si>
+    <t>洪呈婭</t>
+  </si>
+  <si>
+    <t>ryan.hall890@example.com</t>
+  </si>
+  <si>
+    <t>Wu Ningwen</t>
+  </si>
+  <si>
+    <t>吳寧雯</t>
+  </si>
+  <si>
+    <t>olivia.allen567@example.com</t>
+  </si>
+  <si>
+    <t>Pan Weiqi</t>
+  </si>
+  <si>
+    <t>潘威淇</t>
+  </si>
+  <si>
+    <t>tyler.young234@example.com</t>
+  </si>
+  <si>
+    <t>Wu Chengrun</t>
+  </si>
+  <si>
+    <t>巫成潤</t>
+  </si>
+  <si>
+    <t>madison.king678@example.com</t>
+  </si>
+  <si>
+    <t>Gao Chiqi</t>
+  </si>
+  <si>
+    <t>高馳齊</t>
+  </si>
+  <si>
+    <t>alexander.scott012@example.com</t>
+  </si>
+  <si>
+    <t>Lin Chengzhen</t>
+  </si>
+  <si>
+    <t>林丞蓁</t>
+  </si>
+  <si>
+    <t>isabella.adams345@example.com</t>
+  </si>
+  <si>
+    <t>Li Qianyan</t>
+  </si>
+  <si>
+    <t>李千晏</t>
+  </si>
+  <si>
+    <t>charlotte.clark789@example.com</t>
+  </si>
+  <si>
+    <t>Dong Zhengxiang</t>
+  </si>
+  <si>
+    <t>董政湘</t>
+  </si>
+  <si>
+    <t>ethan.harris456@example.com</t>
+  </si>
+  <si>
+    <t>Yuan Jietian</t>
+  </si>
+  <si>
+    <t>袁婕恬</t>
+  </si>
+  <si>
+    <t>grace.lewis001@example.com</t>
+  </si>
+  <si>
+    <t>Wang Xianlan</t>
+  </si>
+  <si>
+    <t>王嫻藍</t>
+  </si>
+  <si>
+    <t>aiden.mitchell234@example.com</t>
+  </si>
+  <si>
+    <t>Qiu Juncheng</t>
+  </si>
+  <si>
+    <t>邱均誠</t>
+  </si>
+  <si>
+    <t>lilly.parker567@example.com</t>
+  </si>
+  <si>
+    <t>Cai Zhiying</t>
+  </si>
+  <si>
+    <t>蔡之瑛</t>
+  </si>
+  <si>
+    <t>lucas.carter890@example.com</t>
+  </si>
+  <si>
+    <t>Liu Xuanyan</t>
+  </si>
+  <si>
+    <t>劉宣晏</t>
+  </si>
+  <si>
+    <t>zoe.wood123@example.com</t>
+  </si>
+  <si>
+    <t>Cheng Jingyun</t>
+  </si>
+  <si>
+    <t>程婧昀</t>
+  </si>
+  <si>
+    <t>noah.thompson456@example.com</t>
+  </si>
+  <si>
+    <t>Xie Muyuan</t>
+  </si>
+  <si>
+    <t>謝木遠</t>
+  </si>
+  <si>
+    <t>sophia.morris789@example.com</t>
+  </si>
+  <si>
+    <t>Lin Xinyu</t>
+  </si>
+  <si>
+    <t>林新雨</t>
+  </si>
+  <si>
+    <t>jackson.rogers012@example.com</t>
+  </si>
+  <si>
+    <t>51234567</t>
+  </si>
+  <si>
+    <t>67890123</t>
+  </si>
+  <si>
+    <t>23456789</t>
+  </si>
+  <si>
+    <t>98765432</t>
+  </si>
+  <si>
+    <t>34567890</t>
+  </si>
+  <si>
+    <t>45678901</t>
+  </si>
+  <si>
+    <t>89012345</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>56789012</t>
+  </si>
+  <si>
+    <t>67891234</t>
+  </si>
+  <si>
+    <t>78902345</t>
+  </si>
+  <si>
+    <t>89013456</t>
+  </si>
+  <si>
+    <t>90124567</t>
+  </si>
+  <si>
+    <t>34905804</t>
+  </si>
+  <si>
+    <t>34561234</t>
+  </si>
+  <si>
+    <t>45672345</t>
+  </si>
+  <si>
+    <t>56783456</t>
+  </si>
+  <si>
+    <t>67894567</t>
+  </si>
+  <si>
+    <t>78905678</t>
+  </si>
+  <si>
+    <t>89016789</t>
+  </si>
+  <si>
+    <t>90127890</t>
+  </si>
+  <si>
+    <t>12348901</t>
+  </si>
+  <si>
+    <t>34568901</t>
+  </si>
+  <si>
+    <t>45679012</t>
+  </si>
+  <si>
+    <t>56780123</t>
+  </si>
+  <si>
+    <t>67892345</t>
+  </si>
+  <si>
+    <t>78903456</t>
+  </si>
+  <si>
+    <t>89014567</t>
+  </si>
+  <si>
+    <t>91234567</t>
   </si>
 </sst>
 </file>
@@ -373,11 +736,11 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -715,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EACDB2-A07A-48A0-83EF-940A4459C1B1}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.08984375" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -725,7 +1088,8 @@
     <col min="2" max="2" width="22.36328125" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.90625" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.54296875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="18" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18" style="3" customWidth="1"/>
     <col min="7" max="7" width="28.36328125" style="3" customWidth="1"/>
     <col min="8" max="16384" width="8.08984375" style="3"/>
   </cols>
@@ -752,11 +1116,21 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="G2" s="6" t="s">
         <v>1</v>
       </c>
@@ -765,11 +1139,21 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="G3" s="6" t="s">
         <v>2</v>
       </c>
@@ -778,300 +1162,580 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="B6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="B8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="B11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="B12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="B13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="B14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="B15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="B16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="B17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="B18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="B19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="B20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
+      <c r="B21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="B22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="B23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="B24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="B25" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+      <c r="B26" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
+      <c r="B27" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
+      <c r="B28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="B29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
+      <c r="B30" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
+      <c r="B31" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="46" spans="5:5" x14ac:dyDescent="0.4">
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="5:5" x14ac:dyDescent="0.4">
-      <c r="E47" s="11" t="s">
+      <c r="E47" s="10" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="g5F4mPe3OwG6VdxYPeFrB6wYE53BzYL0yPDHqbFS6VX1StNmDb7IkYioc8nhz0+8w6+tgNV3UvldJ/HMYNpcyQ==" saltValue="m+5H+qbCy/vXKLmtyc2W3w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="RpSXAt+p2cNp1TH66Unu8TlfHd/Kyc0UxvVUMg4408Ke8wT77ZQqLCtYRl0QZSaBQhYm/gG8dW5msqkgVVt3sQ==" saltValue="k7YZ2aGPjwRX/tt0LNS1Aw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please only input letters and spaces!_x000a_請僅輸入英文字母和空格!" sqref="B2:B31" xr:uid="{71F114F4-8C4B-446B-BBCA-CA68DB44C23C}">
       <formula1>AND(ISTEXT(B2), NOT(ISERROR(MATCH(TRUE, ISNUMBER(FIND(MID(B2,ROW(INDIRECT("1:"&amp;LEN(B2))), 1), "ABCDEFGHIJKLMNOPQRSTUVWXYZabcdefghijklmnopqrstuvwxyz")), 0))))</formula1>
     </dataValidation>
-    <dataValidation type="textLength" imeMode="off" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please input 8 digit number!_x000a_請輸入八位數字!" sqref="D2:D31" xr:uid="{8F92E5BF-5B18-4226-ABBA-A9AAB5E0B2B9}">
+    <dataValidation type="textLength" imeMode="off" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please input 8 digit number!_x000a_請輸入八位數字!" sqref="D3:D31 D2" xr:uid="{8F92E5BF-5B18-4226-ABBA-A9AAB5E0B2B9}">
       <formula1>8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F31" xr:uid="{2220EB65-58D7-4F25-8A57-46F0261ECFA8}">

</xml_diff>